<commit_message>
fix keymap typo & add VIA support format keyboad layout
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmakoto\Desktop\Lenovo_keyboard_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898D9035-4D9D-43E0-A23E-475029C51D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B2A2D0-2B77-4B0B-802C-A2F84DC7CCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{53D0D718-AEE3-4A50-AF55-CF2A7B9629DA}"/>
   </bookViews>
@@ -327,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,14 +336,28 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -566,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,6 +640,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -964,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63EFF70-8428-4F60-83F5-CD61B2B9628D}">
   <dimension ref="B1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1000,10 +1047,10 @@
       <c r="I2" s="18">
         <v>25</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="25">
         <v>23</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="25">
         <v>24</v>
       </c>
       <c r="L2" s="18">
@@ -1012,7 +1059,7 @@
       <c r="M2" s="18">
         <v>29</v>
       </c>
-      <c r="N2" s="18">
+      <c r="N2" s="21">
         <v>32</v>
       </c>
       <c r="O2" s="18">
@@ -1031,7 +1078,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
@@ -1052,10 +1099,10 @@
       <c r="I3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="26" t="s">
         <v>18</v>
       </c>
       <c r="L3" s="6" t="s">
@@ -1064,7 +1111,7 @@
       <c r="M3" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="22" t="s">
         <v>35</v>
       </c>
       <c r="O3" s="6" t="s">
@@ -1109,17 +1156,17 @@
       <c r="I4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="28" t="s">
         <v>32</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>45</v>
       </c>
       <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
+      <c r="N4" s="23"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9" t="s">
@@ -1154,17 +1201,17 @@
       <c r="I5" s="9">
         <v>8</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="27">
         <v>9</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="27">
         <v>0</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="9"/>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="23" t="s">
         <v>39</v>
       </c>
       <c r="O5" s="9" t="s">
@@ -1203,10 +1250,10 @@
       <c r="I6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="27" t="s">
         <v>82</v>
       </c>
       <c r="L6" s="9" t="s">
@@ -1215,7 +1262,7 @@
       <c r="M6" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="N6" s="9"/>
+      <c r="N6" s="23"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
@@ -1250,15 +1297,15 @@
       <c r="I7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="27" t="s">
         <v>29</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
+      <c r="N7" s="23"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
         <v>62</v>
@@ -1295,17 +1342,17 @@
       <c r="I8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="27" t="s">
         <v>19</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>84</v>
       </c>
       <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
+      <c r="N8" s="23"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
@@ -1336,16 +1383,18 @@
       <c r="I9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10" t="s">
+      <c r="J9" s="27"/>
+      <c r="K9" s="28" t="s">
         <v>60</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
+      <c r="M9" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" s="23"/>
+      <c r="O9" s="30"/>
       <c r="P9" s="9" t="s">
         <v>61</v>
       </c>
@@ -1379,20 +1428,18 @@
       <c r="I10" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="9"/>
+      <c r="K10" s="27"/>
       <c r="L10" s="9" t="s">
         <v>55</v>
       </c>
       <c r="M10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9" t="s">
-        <v>89</v>
-      </c>
+      <c r="N10" s="23"/>
+      <c r="O10" s="27"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9" t="s">
         <v>91</v>
@@ -1419,18 +1466,18 @@
       <c r="H11" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="L11" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
       <c r="M11" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="24" t="s">
         <v>77</v>
       </c>
       <c r="O11" s="14" t="s">

</xml_diff>